<commit_message>
Set minimum time to 5 min
</commit_message>
<xml_diff>
--- a/Laktat_Testprotokoll.xlsx
+++ b/Laktat_Testprotokoll.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahocevar/projects/lactate-test-pacemaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{531AA571-CC14-FE4D-8C54-3358E55829D5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{30EE7743-CCC9-4444-84F6-6ED0101949AC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2520" yWindow="-21160" windowWidth="16160" windowHeight="21160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2520" yWindow="-21160" windowWidth="16160" windowHeight="21160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="6-7-8-9-10-11-12 kmh" sheetId="1" r:id="rId1"/>
@@ -493,10 +493,10 @@
     </r>
   </si>
   <si>
-    <t>1 x 400 m, 6 x 800 m</t>
+    <t>4 x 800 m, 3 x 1200 m</t>
   </si>
   <si>
-    <t>4 x 800 m, 2 x 1.200 m</t>
+    <t>3 x 800 m, 3 x 1.200 m</t>
   </si>
 </sst>
 </file>
@@ -2704,8 +2704,8 @@
   </sheetPr>
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2808,8 +2808,8 @@
     </row>
     <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16">
-        <f>400/B10/86400</f>
-        <v>2.7777777777777783E-3</v>
+        <f>800/B10/86400</f>
+        <v>5.5555555555555566E-3</v>
       </c>
       <c r="B10" s="5">
         <f>6/3.6</f>
@@ -2820,7 +2820,7 @@
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
-        <f>800/B11/86400</f>
+        <f t="shared" ref="A11:A16" si="0">800/B11/86400</f>
         <v>4.7619047619047623E-3</v>
       </c>
       <c r="B11" s="5">
@@ -2832,7 +2832,7 @@
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="16">
-        <f>800/B12/86400</f>
+        <f t="shared" si="0"/>
         <v>4.1666666666666666E-3</v>
       </c>
       <c r="B12" s="5">
@@ -2844,7 +2844,7 @@
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="16">
-        <f>800/B13/86400</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037038E-3</v>
       </c>
       <c r="B13" s="5">
@@ -2856,8 +2856,8 @@
     </row>
     <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16">
-        <f>800/B14/86400</f>
-        <v>3.3333333333333335E-3</v>
+        <f>1200/B14/86400</f>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="B14" s="5">
         <f>10/3.6</f>
@@ -2868,8 +2868,8 @@
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16">
-        <f>800/B15/86400</f>
-        <v>3.0303030303030303E-3</v>
+        <f>1200/B15/86400</f>
+        <v>4.5454545454545461E-3</v>
       </c>
       <c r="B15" s="5">
         <f>11/3.6</f>
@@ -2880,8 +2880,8 @@
     </row>
     <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="16">
-        <f>800/B16/86400</f>
-        <v>2.7777777777777783E-3</v>
+        <f>1200/B16/86400</f>
+        <v>4.1666666666666675E-3</v>
       </c>
       <c r="B16" s="5">
         <f>12/3.6</f>
@@ -3189,6 +3189,7 @@
     </row>
     <row r="43" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A42:D42"/>
   </mergeCells>
@@ -3232,8 +3233,8 @@
   </sheetPr>
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3372,8 +3373,8 @@
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="16">
-        <f>800/B13/86400</f>
-        <v>3.0303030303030303E-3</v>
+        <f>1200/B13/86400</f>
+        <v>4.5454545454545461E-3</v>
       </c>
       <c r="B13" s="5">
         <f>11/3.6</f>
@@ -3396,7 +3397,7 @@
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16">
-        <f t="shared" ref="A11:A15" si="0">1200/B15/86400</f>
+        <f t="shared" ref="A15" si="0">1200/B15/86400</f>
         <v>3.5714285714285713E-3</v>
       </c>
       <c r="B15" s="5">
@@ -3705,6 +3706,7 @@
     </row>
     <row r="42" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A41:D41"/>
   </mergeCells>

</xml_diff>

<commit_message>
Update Excel sheet with distance and km/h
</commit_message>
<xml_diff>
--- a/Laktat_Testprotokoll.xlsx
+++ b/Laktat_Testprotokoll.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahocevar/projects/lactate-test-pacemaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{CBE57403-40C6-9846-B381-0FEEAF001B53}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F981FD3D-872E-3246-A071-1464EA450D2C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2520" yWindow="-21160" windowWidth="16160" windowHeight="21160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="16160" windowHeight="20560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="6-7-8-9-10-11-12 kmh" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
   <si>
     <t>2,5 - 3,0/6,0</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -219,33 +219,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>(m/s)</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>Zeit</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(min)</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -498,15 +471,69 @@
   <si>
     <t>4 x 800 m, 3 x 1.200 m</t>
   </si>
+  <si>
+    <r>
+      <t>Geschwindigkeit</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(km/h)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Streckenlänge - Zeit</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(min)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="&quot;&lt; &quot;0"/>
     <numFmt numFmtId="166" formatCode="&quot;&lt; &quot;0.0"/>
+    <numFmt numFmtId="168" formatCode="&quot;800 m - &quot;mm:ss"/>
+    <numFmt numFmtId="169" formatCode="&quot;1.200 m - &quot;mm:ss"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -783,7 +810,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -826,9 +853,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="45" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -874,6 +898,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="161">
@@ -1185,25 +1215,25 @@
                 <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.6666666666666665</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9444444444444444</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2222222222222223</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7777777777777777</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0555555555555554</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.333333333333333</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1369,25 +1399,25 @@
                 <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.6666666666666665</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9444444444444444</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2222222222222223</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7777777777777777</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0555555555555554</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.333333333333333</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1714,22 +1744,22 @@
                 <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.8055555555555556</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2222222222222223</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6388888888888888</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0555555555555554</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.4722222222222223</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.8888888888888888</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1895,22 +1925,22 @@
                 <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.8055555555555556</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2222222222222223</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6388888888888888</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0555555555555554</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.4722222222222223</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.8888888888888888</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2704,8 +2734,8 @@
   </sheetPr>
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2718,65 +2748,65 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="25"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="25"/>
+        <v>16</v>
+      </c>
+      <c r="B2" s="24"/>
       <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="25"/>
+        <v>8</v>
+      </c>
+      <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="25"/>
+        <v>9</v>
+      </c>
+      <c r="B3" s="24"/>
       <c r="C3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="25"/>
+        <v>19</v>
+      </c>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="25"/>
+      <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="25"/>
+      <c r="D5" s="24"/>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="25"/>
+        <v>17</v>
+      </c>
+      <c r="D6" s="24"/>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
@@ -2786,7 +2816,7 @@
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -2794,10 +2824,10 @@
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>5</v>
@@ -2807,88 +2837,88 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16">
+      <c r="A10" s="30">
         <f>800/B10/86400</f>
-        <v>5.5555555555555566E-3</v>
+        <v>1.54320987654321E-3</v>
       </c>
       <c r="B10" s="5">
-        <f>6/3.6</f>
-        <v>1.6666666666666665</v>
-      </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="28"/>
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="27"/>
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16">
+      <c r="A11" s="30">
         <f t="shared" ref="A11:A13" si="0">800/B11/86400</f>
-        <v>4.7619047619047623E-3</v>
+        <v>1.3227513227513229E-3</v>
       </c>
       <c r="B11" s="5">
-        <f>7/3.6</f>
-        <v>1.9444444444444444</v>
-      </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="28"/>
+        <f>7</f>
+        <v>7</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="27"/>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16">
+      <c r="A12" s="30">
         <f t="shared" si="0"/>
-        <v>4.1666666666666666E-3</v>
+        <v>1.1574074074074073E-3</v>
       </c>
       <c r="B12" s="5">
-        <f>8/3.6</f>
-        <v>2.2222222222222223</v>
-      </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="28"/>
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="27"/>
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16">
+      <c r="A13" s="30">
         <f t="shared" si="0"/>
-        <v>3.7037037037037038E-3</v>
+        <v>1.0288065843621398E-3</v>
       </c>
       <c r="B13" s="5">
-        <f>9/3.6</f>
-        <v>2.5</v>
-      </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="28"/>
+        <f>9</f>
+        <v>9</v>
+      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="27"/>
     </row>
     <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16">
+      <c r="A14" s="31">
         <f>1200/B14/86400</f>
-        <v>5.0000000000000001E-3</v>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="B14" s="5">
-        <f>10/3.6</f>
-        <v>2.7777777777777777</v>
-      </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="28"/>
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="27"/>
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16">
+      <c r="A15" s="31">
         <f>1200/B15/86400</f>
-        <v>4.5454545454545461E-3</v>
+        <v>1.2626262626262627E-3</v>
       </c>
       <c r="B15" s="5">
-        <f>11/3.6</f>
-        <v>3.0555555555555554</v>
-      </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="28"/>
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="C15" s="26"/>
+      <c r="D15" s="27"/>
     </row>
     <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="16">
+      <c r="A16" s="31">
         <f>1200/B16/86400</f>
-        <v>4.1666666666666675E-3</v>
+        <v>1.1574074074074073E-3</v>
       </c>
       <c r="B16" s="5">
-        <f>12/3.6</f>
-        <v>3.333333333333333</v>
-      </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="28"/>
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="27"/>
     </row>
     <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9"/>
@@ -2917,7 +2947,7 @@
     <row r="21" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
-      <c r="C21" s="24"/>
+      <c r="C21" s="23"/>
       <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -2974,11 +3004,11 @@
         <f>B40</f>
         <v>4</v>
       </c>
-      <c r="C26" s="23" t="e">
+      <c r="C26" s="22" t="e">
         <f ca="1">FORECAST(1.5,OFFSET(KnownY,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,1.5),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,1.5),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D26" s="24" t="e">
+      <c r="D26" s="23" t="e">
         <f ca="1">FORECAST(1.5,OFFSET(KnownV,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,1.5),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,1.5),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
@@ -2992,11 +3022,11 @@
         <f>B40</f>
         <v>4</v>
       </c>
-      <c r="C27" s="23" t="e">
+      <c r="C27" s="22" t="e">
         <f ca="1">FORECAST(2.5,OFFSET(KnownY,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,2.5),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,2.5),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D27" s="24" t="e">
+      <c r="D27" s="23" t="e">
         <f ca="1">FORECAST(2.5,OFFSET(KnownV,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,2.5),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,2.5),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
@@ -3009,11 +3039,11 @@
       <c r="B28" s="14">
         <v>0</v>
       </c>
-      <c r="C28" s="23" t="e">
+      <c r="C28" s="22" t="e">
         <f ca="1">FORECAST(3,OFFSET(KnownY,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,3),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,3),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D28" s="24" t="e">
+      <c r="D28" s="23" t="e">
         <f ca="1">FORECAST(3,OFFSET(KnownV,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,3),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,3),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
@@ -3027,11 +3057,11 @@
         <f ca="1">C40</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C29" s="23" t="e">
+      <c r="C29" s="22" t="e">
         <f ca="1">FORECAST(6,OFFSET(KnownY,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,6),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,6),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D29" s="24" t="e">
+      <c r="D29" s="23" t="e">
         <f ca="1">FORECAST(6,OFFSET(KnownV,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,6),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,6),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
@@ -3044,7 +3074,7 @@
     </row>
     <row r="31" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -3066,48 +3096,48 @@
     </row>
     <row r="33" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="19" t="str">
+        <v>25</v>
+      </c>
+      <c r="C33" s="18" t="str">
         <f ca="1">"&lt; "&amp;IFERROR(TEXT(C26,"0"),"?")</f>
         <v>&lt; ?</v>
       </c>
-      <c r="D33" s="20" t="str">
+      <c r="D33" s="19" t="str">
         <f ca="1">"&lt; "&amp;IFERROR(TEXT(D26,"0,0"),"?")</f>
         <v>&lt; ?</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="19" t="str">
+        <v>26</v>
+      </c>
+      <c r="C34" s="18" t="str">
         <f ca="1">IFERROR(TEXT(C26,"0"),"?")&amp;" - "&amp;IFERROR(TEXT(C27,"0"),"?")</f>
         <v>? - ?</v>
       </c>
-      <c r="D34" s="19" t="str">
+      <c r="D34" s="18" t="str">
         <f ca="1">IFERROR(TEXT(D26,"0,0"),"?")&amp;" - "&amp;IFERROR(TEXT(D27,"0,0"),"?")</f>
         <v>? - ?</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B35" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C35" s="19" t="str">
+      <c r="C35" s="18" t="str">
         <f ca="1">IFERROR(TEXT(C27,"0"),"?")&amp;" - "&amp;IFERROR(TEXT(C28,"0"),"?")&amp;"/"&amp;IFERROR(TEXT(C29,"0"),"?")</f>
         <v>? - ?/?</v>
       </c>
-      <c r="D35" s="19" t="str">
+      <c r="D35" s="18" t="str">
         <f ca="1">IFERROR(TEXT(D27,"0,0"),"?")&amp;" - "&amp;IFERROR(TEXT(D28,"0,0"),"?")&amp;"/"&amp;IFERROR(TEXT(D29,"0,0"),"?")</f>
         <v>? - ?/?</v>
       </c>
@@ -3145,11 +3175,11 @@
       <c r="B39" s="5">
         <v>2</v>
       </c>
-      <c r="C39" s="21" t="e">
+      <c r="C39" s="20" t="e">
         <f ca="1">FORECAST(2,OFFSET(KnownY,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,2),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,2),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D39" s="22" t="e">
+      <c r="D39" s="21" t="e">
         <f ca="1">FORECAST(2,OFFSET(KnownV,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,2),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,2),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
@@ -3161,31 +3191,31 @@
       <c r="B40" s="5">
         <v>4</v>
       </c>
-      <c r="C40" s="21" t="e">
+      <c r="C40" s="20" t="e">
         <f ca="1">FORECAST(4,OFFSET(KnownY,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,4),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,4),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D40" s="22" t="e">
+      <c r="D40" s="21" t="e">
         <f ca="1">FORECAST(4,OFFSET(KnownV,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,4),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,4),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:12" ht="56" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B42" s="30"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="17"/>
-      <c r="K42" s="17"/>
-      <c r="L42" s="17"/>
+      <c r="A42" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
     </row>
     <row r="43" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -3233,8 +3263,8 @@
   </sheetPr>
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3247,65 +3277,65 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="25"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="25"/>
+        <v>16</v>
+      </c>
+      <c r="B2" s="24"/>
       <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="25"/>
+        <v>8</v>
+      </c>
+      <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="25"/>
+        <v>9</v>
+      </c>
+      <c r="B3" s="24"/>
       <c r="C3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="25"/>
+        <v>19</v>
+      </c>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="25"/>
+      <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="25"/>
+      <c r="D5" s="24"/>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="25"/>
+        <v>17</v>
+      </c>
+      <c r="D6" s="24"/>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
@@ -3315,7 +3345,7 @@
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -3323,10 +3353,10 @@
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>5</v>
@@ -3336,76 +3366,76 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16">
+      <c r="A10" s="30">
         <f>800/B10/86400</f>
-        <v>5.1282051282051282E-3</v>
+        <v>1.4245014245014246E-3</v>
       </c>
       <c r="B10" s="5">
-        <f>6.5/3.6</f>
-        <v>1.8055555555555556</v>
-      </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="28"/>
+        <f>6.5</f>
+        <v>6.5</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="27"/>
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16">
+      <c r="A11" s="30">
         <f>800/B11/86400</f>
-        <v>4.1666666666666666E-3</v>
+        <v>1.1574074074074073E-3</v>
       </c>
       <c r="B11" s="5">
-        <f>8/3.6</f>
-        <v>2.2222222222222223</v>
-      </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="28"/>
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="27"/>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16">
+      <c r="A12" s="30">
         <f>800/B12/86400</f>
-        <v>3.5087719298245619E-3</v>
+        <v>9.7465886939571156E-4</v>
       </c>
       <c r="B12" s="5">
-        <f>9.5/3.6</f>
-        <v>2.6388888888888888</v>
-      </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="28"/>
+        <f>9.5</f>
+        <v>9.5</v>
+      </c>
+      <c r="C12" s="26"/>
+      <c r="D12" s="27"/>
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16">
+      <c r="A13" s="31">
         <f>1200/B13/86400</f>
-        <v>4.5454545454545461E-3</v>
+        <v>1.2626262626262627E-3</v>
       </c>
       <c r="B13" s="5">
-        <f>11/3.6</f>
-        <v>3.0555555555555554</v>
-      </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="28"/>
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="27"/>
     </row>
     <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16">
+      <c r="A14" s="31">
         <f>1200/B14/86400</f>
-        <v>3.9999999999999992E-3</v>
+        <v>1.1111111111111111E-3</v>
       </c>
       <c r="B14" s="5">
-        <f>12.5/3.6</f>
-        <v>3.4722222222222223</v>
-      </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="28"/>
+        <f>12.5</f>
+        <v>12.5</v>
+      </c>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16">
+      <c r="A15" s="31">
         <f t="shared" ref="A15" si="0">1200/B15/86400</f>
-        <v>3.5714285714285713E-3</v>
+        <v>9.9206349206349201E-4</v>
       </c>
       <c r="B15" s="5">
-        <f>14/3.6</f>
-        <v>3.8888888888888888</v>
-      </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="28"/>
+        <f>14</f>
+        <v>14</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="27"/>
     </row>
     <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
@@ -3434,7 +3464,7 @@
     <row r="20" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="24"/>
+      <c r="C20" s="23"/>
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -3491,11 +3521,11 @@
         <f>B39</f>
         <v>4</v>
       </c>
-      <c r="C25" s="23" t="e">
+      <c r="C25" s="22" t="e">
         <f ca="1">FORECAST(1.5,OFFSET(KnownY,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,1.5),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,1.5),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D25" s="24" t="e">
+      <c r="D25" s="23" t="e">
         <f ca="1">FORECAST(1.5,OFFSET(KnownV,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,1.5),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,1.5),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
@@ -3509,11 +3539,11 @@
         <f>B39</f>
         <v>4</v>
       </c>
-      <c r="C26" s="23" t="e">
+      <c r="C26" s="22" t="e">
         <f ca="1">FORECAST(2.5,OFFSET(KnownY,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,2.5),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,2.5),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D26" s="24" t="e">
+      <c r="D26" s="23" t="e">
         <f ca="1">FORECAST(2.5,OFFSET(KnownV,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,2.5),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,2.5),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
@@ -3526,11 +3556,11 @@
       <c r="B27" s="14">
         <v>0</v>
       </c>
-      <c r="C27" s="23" t="e">
+      <c r="C27" s="22" t="e">
         <f ca="1">FORECAST(3,OFFSET(KnownY,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,3),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,3),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D27" s="24" t="e">
+      <c r="D27" s="23" t="e">
         <f ca="1">FORECAST(3,OFFSET(KnownV,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,3),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,3),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
@@ -3544,11 +3574,11 @@
         <f ca="1">C39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C28" s="23" t="e">
+      <c r="C28" s="22" t="e">
         <f ca="1">FORECAST(6,OFFSET(KnownY,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,6),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,6),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D28" s="24" t="e">
+      <c r="D28" s="23" t="e">
         <f ca="1">FORECAST(6,OFFSET(KnownV,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,6),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,6),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
@@ -3561,7 +3591,7 @@
     </row>
     <row r="30" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -3583,48 +3613,48 @@
     </row>
     <row r="32" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="19" t="str">
+        <v>25</v>
+      </c>
+      <c r="C32" s="18" t="str">
         <f ca="1">"&lt; "&amp;IFERROR(TEXT(C25,"0"),"?")</f>
         <v>&lt; ?</v>
       </c>
-      <c r="D32" s="20" t="str">
+      <c r="D32" s="19" t="str">
         <f ca="1">"&lt; "&amp;IFERROR(TEXT(D25,"0,0"),"?")</f>
         <v>&lt; ?</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="19" t="str">
+        <v>26</v>
+      </c>
+      <c r="C33" s="18" t="str">
         <f ca="1">IFERROR(TEXT(C25,"0"),"?")&amp;" - "&amp;IFERROR(TEXT(C26,"0"),"?")</f>
         <v>? - ?</v>
       </c>
-      <c r="D33" s="19" t="str">
+      <c r="D33" s="18" t="str">
         <f ca="1">IFERROR(TEXT(D25,"0,0"),"?")&amp;" - "&amp;IFERROR(TEXT(D26,"0,0"),"?")</f>
         <v>? - ?</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="19" t="str">
+      <c r="C34" s="18" t="str">
         <f ca="1">IFERROR(TEXT(C26,"0"),"?")&amp;" - "&amp;IFERROR(TEXT(C27,"0"),"?")&amp;"/"&amp;IFERROR(TEXT(C28,"0"),"?")</f>
         <v>? - ?/?</v>
       </c>
-      <c r="D34" s="19" t="str">
+      <c r="D34" s="18" t="str">
         <f ca="1">IFERROR(TEXT(D26,"0,0"),"?")&amp;" - "&amp;IFERROR(TEXT(D27,"0,0"),"?")&amp;"/"&amp;IFERROR(TEXT(D28,"0,0"),"?")</f>
         <v>? - ?/?</v>
       </c>
@@ -3662,11 +3692,11 @@
       <c r="B38" s="5">
         <v>2</v>
       </c>
-      <c r="C38" s="21" t="e">
+      <c r="C38" s="20" t="e">
         <f ca="1">FORECAST(2,OFFSET(KnownY,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,2),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,2),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D38" s="22" t="e">
+      <c r="D38" s="21" t="e">
         <f ca="1">FORECAST(2,OFFSET(KnownV,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,2),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,2),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
@@ -3678,31 +3708,31 @@
       <c r="B39" s="5">
         <v>4</v>
       </c>
-      <c r="C39" s="21" t="e">
+      <c r="C39" s="20" t="e">
         <f ca="1">FORECAST(4,OFFSET(KnownY,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,4),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,4),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D39" s="22" t="e">
+      <c r="D39" s="21" t="e">
         <f ca="1">FORECAST(4,OFFSET(KnownV,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,4),KnownX,1)-1,0),0,2),OFFSET(KnownX,IFERROR(MATCH(MIN(MAX(KnownX)-0.0001,4),KnownX,1)-1,0),0,2))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:12" ht="56" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
+      <c r="A41" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
     </row>
     <row r="42" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>

</xml_diff>

<commit_message>
Fix km/h vs. m/s bug
</commit_message>
<xml_diff>
--- a/Laktat_Testprotokoll.xlsx
+++ b/Laktat_Testprotokoll.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahocevar/projects/lactate-test-pacemaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F981FD3D-872E-3246-A071-1464EA450D2C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{22BC4EC4-0624-544F-9123-953C9436627B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="16160" windowHeight="20560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="16160" windowHeight="20560" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="6-7-8-9-10-11-12 kmh" sheetId="1" r:id="rId1"/>
@@ -473,32 +473,6 @@
   </si>
   <si>
     <r>
-      <t>Geschwindigkeit</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(km/h)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Streckenlänge - Zeit</t>
     </r>
     <r>
@@ -521,6 +495,32 @@
         <scheme val="minor"/>
       </rPr>
       <t>(min)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Geschwindigkeit</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(m/s)</t>
     </r>
   </si>
 </sst>
@@ -532,8 +532,8 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="&quot;&lt; &quot;0"/>
     <numFmt numFmtId="166" formatCode="&quot;&lt; &quot;0.0"/>
-    <numFmt numFmtId="168" formatCode="&quot;800 m - &quot;mm:ss"/>
-    <numFmt numFmtId="169" formatCode="&quot;1.200 m - &quot;mm:ss"/>
+    <numFmt numFmtId="167" formatCode="&quot;800 m - &quot;mm:ss"/>
+    <numFmt numFmtId="168" formatCode="&quot;1.200 m - &quot;mm:ss"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -893,17 +893,17 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="161">
@@ -1215,25 +1215,25 @@
                 <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>1.6666666666666665</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>1.9444444444444444</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>2.2222222222222223</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>2.7777777777777777</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>3.0555555555555554</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>3.333333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1399,25 +1399,25 @@
                 <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>1.6666666666666665</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>1.9444444444444444</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>2.2222222222222223</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>2.7777777777777777</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>3.0555555555555554</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>3.333333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1744,22 +1744,22 @@
                 <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6.5</c:v>
+                  <c:v>1.8055555555555556</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>2.2222222222222223</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.5</c:v>
+                  <c:v>2.6388888888888888</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>3.0555555555555554</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.5</c:v>
+                  <c:v>3.4722222222222223</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>3.8888888888888888</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1925,22 +1925,22 @@
                 <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6.5</c:v>
+                  <c:v>1.8055555555555556</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>2.2222222222222223</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.5</c:v>
+                  <c:v>2.6388888888888888</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>3.0555555555555554</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.5</c:v>
+                  <c:v>3.4722222222222223</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>3.8888888888888888</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2734,8 +2734,8 @@
   </sheetPr>
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2824,10 +2824,10 @@
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>30</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>5</v>
@@ -2837,85 +2837,85 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="30">
+      <c r="A10" s="28">
         <f>800/B10/86400</f>
-        <v>1.54320987654321E-3</v>
+        <v>5.5555555555555566E-3</v>
       </c>
       <c r="B10" s="5">
-        <f>6</f>
-        <v>6</v>
+        <f>6/3.6</f>
+        <v>1.6666666666666665</v>
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="27"/>
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="30">
+      <c r="A11" s="28">
         <f t="shared" ref="A11:A13" si="0">800/B11/86400</f>
-        <v>1.3227513227513229E-3</v>
+        <v>4.7619047619047623E-3</v>
       </c>
       <c r="B11" s="5">
-        <f>7</f>
-        <v>7</v>
+        <f>7/3.6</f>
+        <v>1.9444444444444444</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="27"/>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="30">
+      <c r="A12" s="28">
         <f t="shared" si="0"/>
-        <v>1.1574074074074073E-3</v>
+        <v>4.1666666666666666E-3</v>
       </c>
       <c r="B12" s="5">
-        <f>8</f>
-        <v>8</v>
+        <f>8/3.6</f>
+        <v>2.2222222222222223</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="27"/>
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="30">
+      <c r="A13" s="28">
         <f t="shared" si="0"/>
-        <v>1.0288065843621398E-3</v>
+        <v>3.7037037037037038E-3</v>
       </c>
       <c r="B13" s="5">
-        <f>9</f>
-        <v>9</v>
+        <f>9/3.6</f>
+        <v>2.5</v>
       </c>
       <c r="C13" s="26"/>
       <c r="D13" s="27"/>
     </row>
     <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="31">
+      <c r="A14" s="29">
         <f>1200/B14/86400</f>
-        <v>1.3888888888888889E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="B14" s="5">
-        <f>10</f>
-        <v>10</v>
+        <f>10/3.6</f>
+        <v>2.7777777777777777</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="27"/>
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="31">
+      <c r="A15" s="29">
         <f>1200/B15/86400</f>
-        <v>1.2626262626262627E-3</v>
+        <v>4.5454545454545461E-3</v>
       </c>
       <c r="B15" s="5">
-        <f>11</f>
-        <v>11</v>
+        <f>11/3.6</f>
+        <v>3.0555555555555554</v>
       </c>
       <c r="C15" s="26"/>
       <c r="D15" s="27"/>
     </row>
     <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="31">
+      <c r="A16" s="29">
         <f>1200/B16/86400</f>
-        <v>1.1574074074074073E-3</v>
+        <v>4.1666666666666675E-3</v>
       </c>
       <c r="B16" s="5">
-        <f>12</f>
-        <v>12</v>
+        <f>12/3.6</f>
+        <v>3.333333333333333</v>
       </c>
       <c r="C16" s="25"/>
       <c r="D16" s="27"/>
@@ -3202,12 +3202,12 @@
     </row>
     <row r="41" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:12" ht="56" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
       <c r="E42" s="16"/>
       <c r="F42" s="16"/>
       <c r="G42" s="16"/>
@@ -3219,7 +3219,6 @@
     </row>
     <row r="43" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A42:D42"/>
   </mergeCells>
@@ -3263,8 +3262,8 @@
   </sheetPr>
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3353,10 +3352,10 @@
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>30</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>5</v>
@@ -3366,73 +3365,73 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="30">
+      <c r="A10" s="28">
         <f>800/B10/86400</f>
-        <v>1.4245014245014246E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="B10" s="5">
-        <f>6.5</f>
-        <v>6.5</v>
+        <f>6.5/3.6</f>
+        <v>1.8055555555555556</v>
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="27"/>
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="30">
+      <c r="A11" s="28">
         <f>800/B11/86400</f>
-        <v>1.1574074074074073E-3</v>
+        <v>4.1666666666666666E-3</v>
       </c>
       <c r="B11" s="5">
-        <f>8</f>
-        <v>8</v>
+        <f>8/3.6</f>
+        <v>2.2222222222222223</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="27"/>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="30">
+      <c r="A12" s="28">
         <f>800/B12/86400</f>
-        <v>9.7465886939571156E-4</v>
+        <v>3.5087719298245619E-3</v>
       </c>
       <c r="B12" s="5">
-        <f>9.5</f>
-        <v>9.5</v>
+        <f>9.5/3.6</f>
+        <v>2.6388888888888888</v>
       </c>
       <c r="C12" s="26"/>
       <c r="D12" s="27"/>
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="31">
+      <c r="A13" s="29">
         <f>1200/B13/86400</f>
-        <v>1.2626262626262627E-3</v>
+        <v>4.5454545454545461E-3</v>
       </c>
       <c r="B13" s="5">
-        <f>11</f>
-        <v>11</v>
+        <f>11/3.6</f>
+        <v>3.0555555555555554</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="27"/>
     </row>
     <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="31">
+      <c r="A14" s="29">
         <f>1200/B14/86400</f>
-        <v>1.1111111111111111E-3</v>
+        <v>3.9999999999999992E-3</v>
       </c>
       <c r="B14" s="5">
-        <f>12.5</f>
-        <v>12.5</v>
+        <f>12.5/3.6</f>
+        <v>3.4722222222222223</v>
       </c>
       <c r="C14" s="26"/>
       <c r="D14" s="27"/>
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="31">
+      <c r="A15" s="29">
         <f t="shared" ref="A15" si="0">1200/B15/86400</f>
-        <v>9.9206349206349201E-4</v>
+        <v>3.5714285714285713E-3</v>
       </c>
       <c r="B15" s="5">
-        <f>14</f>
-        <v>14</v>
+        <f>14/3.6</f>
+        <v>3.8888888888888888</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="27"/>
@@ -3719,12 +3718,12 @@
     </row>
     <row r="40" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:12" ht="56" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
+      <c r="A41" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
       <c r="E41" s="17"/>
       <c r="F41" s="17"/>
       <c r="G41" s="17"/>
@@ -3736,7 +3735,6 @@
     </row>
     <row r="42" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A41:D41"/>
   </mergeCells>

</xml_diff>